<commit_message>
new 'christmas tree' project
</commit_message>
<xml_diff>
--- a/Kalkulator rezystancji.xlsx
+++ b/Kalkulator rezystancji.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="11292" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -139,8 +139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,12 +233,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -249,6 +243,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -287,7 +287,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -361,7 +361,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,27 +393,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -445,24 +427,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -638,121 +602,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="2.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="1.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="2.42578125" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="37.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="2.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="1.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="2.44140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:20" ht="32.4" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="7">
+      <c r="B7" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
+        <f>(B3-B5)/((B6/1000)*B4)</f>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3">
+        <f>(B3-B5)*((B6*B4)/1000)</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <f>(4.2-0.7)/((B6*B4)/1000/B7)</f>
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="5">
-        <f>(B3-B5)/((B6/1000)*B4)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5">
-        <f>(B3-B5)*((B6*B4)/1000)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="4">
-        <f>(4.2-0.7)/((B6*B4)/1000/B7)</f>
-        <v>700</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <f>(4.2-0.7)*((B6*B4)/1000/B7)</f>
-        <v>1.7500000000000002E-2</v>
+        <v>2.8E-3</v>
       </c>
     </row>
   </sheetData>
@@ -766,12 +730,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -779,12 +743,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>